<commit_message>
added hair chord data and getParameterAsync()
</commit_message>
<xml_diff>
--- a/data/ChordData.xlsx
+++ b/data/ChordData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16620" firstSheet="5" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16620" firstSheet="5" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Intro" sheetId="23" r:id="rId1"/>
@@ -19,12 +19,13 @@
     <sheet name="Cleaned Up Phone Data" sheetId="11" r:id="rId5"/>
     <sheet name="Phone Matrix" sheetId="6" r:id="rId6"/>
     <sheet name="Phone Matrix-Tableau" sheetId="13" r:id="rId7"/>
-    <sheet name="Phone Data Ready" sheetId="8" r:id="rId8"/>
-    <sheet name="Raw Uber Data" sheetId="16" r:id="rId9"/>
-    <sheet name="Uber Matrix Cleanup" sheetId="17" r:id="rId10"/>
-    <sheet name="Uber Matrix" sheetId="18" r:id="rId11"/>
-    <sheet name="Uber Matrix-Tableau" sheetId="22" r:id="rId12"/>
-    <sheet name="Uber Data Ready" sheetId="21" r:id="rId13"/>
+    <sheet name="Hair Matrix Tableau" sheetId="24" r:id="rId8"/>
+    <sheet name="Phone Data Ready" sheetId="8" r:id="rId9"/>
+    <sheet name="Raw Uber Data" sheetId="16" r:id="rId10"/>
+    <sheet name="Uber Matrix Cleanup" sheetId="17" r:id="rId11"/>
+    <sheet name="Uber Matrix" sheetId="18" r:id="rId12"/>
+    <sheet name="Uber Matrix-Tableau" sheetId="22" r:id="rId13"/>
+    <sheet name="Uber Data Ready" sheetId="21" r:id="rId14"/>
   </sheets>
   <calcPr calcId="125725" concurrentCalc="0"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8085" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8120" uniqueCount="144">
   <si>
     <t>HTC</t>
   </si>
@@ -447,6 +448,27 @@
   </si>
   <si>
     <t>Population1</t>
+  </si>
+  <si>
+    <t>has</t>
+  </si>
+  <si>
+    <t>prefers</t>
+  </si>
+  <si>
+    <t>count</t>
+  </si>
+  <si>
+    <t>black</t>
+  </si>
+  <si>
+    <t>red</t>
+  </si>
+  <si>
+    <t>blonde</t>
+  </si>
+  <si>
+    <t>brown</t>
   </si>
 </sst>
 </file>
@@ -1976,6 +1998,649 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E40"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:E40"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6">
+        <v>37.724400000000003</v>
+      </c>
+      <c r="C6">
+        <v>-122.42100000000001</v>
+      </c>
+      <c r="D6">
+        <v>8.3884E-2</v>
+      </c>
+      <c r="E6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7">
+        <v>37.710700000000003</v>
+      </c>
+      <c r="C7">
+        <v>-122.4372</v>
+      </c>
+      <c r="D7">
+        <v>5.8438999999999998E-2</v>
+      </c>
+      <c r="E7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8">
+        <v>37.802100000000003</v>
+      </c>
+      <c r="C8">
+        <v>-122.43689999999999</v>
+      </c>
+      <c r="D8">
+        <v>0.40364</v>
+      </c>
+      <c r="E8" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>56</v>
+      </c>
+      <c r="B9">
+        <v>37.792999999999999</v>
+      </c>
+      <c r="C9">
+        <v>-122.416</v>
+      </c>
+      <c r="D9">
+        <v>0.33259</v>
+      </c>
+      <c r="E9" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>57</v>
+      </c>
+      <c r="B10">
+        <v>37.804499999999997</v>
+      </c>
+      <c r="C10">
+        <v>-122.4076</v>
+      </c>
+      <c r="D10">
+        <v>0.28783999999999998</v>
+      </c>
+      <c r="E10" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>58</v>
+      </c>
+      <c r="B11">
+        <v>37.792400000000001</v>
+      </c>
+      <c r="C11">
+        <v>-122.43519999999999</v>
+      </c>
+      <c r="D11">
+        <v>0.33382000000000001</v>
+      </c>
+      <c r="E11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>59</v>
+      </c>
+      <c r="B12">
+        <v>37.786799999999999</v>
+      </c>
+      <c r="C12">
+        <v>-122.4538</v>
+      </c>
+      <c r="D12">
+        <v>0.19964999999999999</v>
+      </c>
+      <c r="E12" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>60</v>
+      </c>
+      <c r="B13">
+        <v>37.801400000000001</v>
+      </c>
+      <c r="C13">
+        <v>-122.4182</v>
+      </c>
+      <c r="D13">
+        <v>0.34165000000000001</v>
+      </c>
+      <c r="E13" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>61</v>
+      </c>
+      <c r="B14">
+        <v>37.714399999999998</v>
+      </c>
+      <c r="C14">
+        <v>-122.4113</v>
+      </c>
+      <c r="D14">
+        <v>6.4773999999999998E-2</v>
+      </c>
+      <c r="E14" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>63</v>
+      </c>
+      <c r="B15">
+        <v>37.7423</v>
+      </c>
+      <c r="C15">
+        <v>-122.4423</v>
+      </c>
+      <c r="D15">
+        <v>7.4148000000000006E-2</v>
+      </c>
+      <c r="E15" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>65</v>
+      </c>
+      <c r="B16">
+        <v>37.7378</v>
+      </c>
+      <c r="C16">
+        <v>-122.4316</v>
+      </c>
+      <c r="D16">
+        <v>0.1226</v>
+      </c>
+      <c r="E16" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>66</v>
+      </c>
+      <c r="B17">
+        <v>37.758400000000002</v>
+      </c>
+      <c r="C17">
+        <v>-122.4654</v>
+      </c>
+      <c r="D17">
+        <v>0.18995000000000001</v>
+      </c>
+      <c r="E17" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>67</v>
+      </c>
+      <c r="B18">
+        <v>37.722499999999997</v>
+      </c>
+      <c r="C18">
+        <v>-122.4885</v>
+      </c>
+      <c r="D18">
+        <v>9.2602000000000004E-2</v>
+      </c>
+      <c r="E18" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>68</v>
+      </c>
+      <c r="B19">
+        <v>37.7239</v>
+      </c>
+      <c r="C19">
+        <v>-122.4439</v>
+      </c>
+      <c r="D19">
+        <v>0.10242</v>
+      </c>
+      <c r="E19" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>69</v>
+      </c>
+      <c r="B20">
+        <v>37.737299999999998</v>
+      </c>
+      <c r="C20">
+        <v>-122.4589</v>
+      </c>
+      <c r="D20">
+        <v>0.12472999999999999</v>
+      </c>
+      <c r="E20" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>70</v>
+      </c>
+      <c r="B21">
+        <v>37.729999999999997</v>
+      </c>
+      <c r="C21">
+        <v>-122.38549999999999</v>
+      </c>
+      <c r="D21">
+        <v>0.10309</v>
+      </c>
+      <c r="E21" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>72</v>
+      </c>
+      <c r="B22">
+        <v>37.739899999999999</v>
+      </c>
+      <c r="C22">
+        <v>-122.4169</v>
+      </c>
+      <c r="D22">
+        <v>0.20043</v>
+      </c>
+      <c r="E22" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>73</v>
+      </c>
+      <c r="B23">
+        <v>37.7624</v>
+      </c>
+      <c r="C23">
+        <v>-122.4348</v>
+      </c>
+      <c r="D23">
+        <v>0.34092</v>
+      </c>
+      <c r="E23" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>74</v>
+      </c>
+      <c r="B24">
+        <v>37.769199999999998</v>
+      </c>
+      <c r="C24">
+        <v>-122.44629999999999</v>
+      </c>
+      <c r="D24">
+        <v>0.29559000000000002</v>
+      </c>
+      <c r="E24" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>75</v>
+      </c>
+      <c r="B25">
+        <v>37.758899999999997</v>
+      </c>
+      <c r="C25">
+        <v>-122.4153</v>
+      </c>
+      <c r="D25">
+        <v>0.42582999999999999</v>
+      </c>
+      <c r="E25" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>76</v>
+      </c>
+      <c r="B26">
+        <v>37.749299999999998</v>
+      </c>
+      <c r="C26">
+        <v>-122.43300000000001</v>
+      </c>
+      <c r="D26">
+        <v>0.25158000000000003</v>
+      </c>
+      <c r="E26" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>77</v>
+      </c>
+      <c r="B27">
+        <v>37.741100000000003</v>
+      </c>
+      <c r="C27">
+        <v>-122.4892</v>
+      </c>
+      <c r="D27">
+        <v>9.2271000000000006E-2</v>
+      </c>
+      <c r="E27" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>78</v>
+      </c>
+      <c r="B28">
+        <v>37.758299999999998</v>
+      </c>
+      <c r="C28">
+        <v>-122.393</v>
+      </c>
+      <c r="D28">
+        <v>0.26352999999999999</v>
+      </c>
+      <c r="E28" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>79</v>
+      </c>
+      <c r="B29">
+        <v>37.776400000000002</v>
+      </c>
+      <c r="C29">
+        <v>-122.3994</v>
+      </c>
+      <c r="D29">
+        <v>0.55315999999999999</v>
+      </c>
+      <c r="E29" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>80</v>
+      </c>
+      <c r="B30">
+        <v>37.752000000000002</v>
+      </c>
+      <c r="C30">
+        <v>-122.45</v>
+      </c>
+      <c r="D30">
+        <v>0.13105</v>
+      </c>
+      <c r="E30" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>81</v>
+      </c>
+      <c r="B31">
+        <v>37.7804</v>
+      </c>
+      <c r="C31">
+        <v>-122.4332</v>
+      </c>
+      <c r="D31">
+        <v>0.41192000000000001</v>
+      </c>
+      <c r="E31" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>82</v>
+      </c>
+      <c r="B32">
+        <v>37.780200000000001</v>
+      </c>
+      <c r="C32">
+        <v>-122.4652</v>
+      </c>
+      <c r="D32">
+        <v>0.21193999999999999</v>
+      </c>
+      <c r="E32" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>84</v>
+      </c>
+      <c r="B33">
+        <v>37.777999999999999</v>
+      </c>
+      <c r="C33">
+        <v>-122.4928</v>
+      </c>
+      <c r="D33">
+        <v>0.18915999999999999</v>
+      </c>
+      <c r="E33" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>85</v>
+      </c>
+      <c r="B34">
+        <v>37.755299999999998</v>
+      </c>
+      <c r="C34">
+        <v>-122.49379999999999</v>
+      </c>
+      <c r="D34">
+        <v>0.12363</v>
+      </c>
+      <c r="E34" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>86</v>
+      </c>
+      <c r="B35">
+        <v>37.784100000000002</v>
+      </c>
+      <c r="C35">
+        <v>-122.5009</v>
+      </c>
+      <c r="D35">
+        <v>9.1937000000000005E-2</v>
+      </c>
+      <c r="E35" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>87</v>
+      </c>
+      <c r="B36">
+        <v>37.768900000000002</v>
+      </c>
+      <c r="C36">
+        <v>-122.4828</v>
+      </c>
+      <c r="D36">
+        <v>0.15941</v>
+      </c>
+      <c r="E36" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>88</v>
+      </c>
+      <c r="B37">
+        <v>37.7941</v>
+      </c>
+      <c r="C37">
+        <v>-122.407</v>
+      </c>
+      <c r="D37">
+        <v>0.24273</v>
+      </c>
+      <c r="E37" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>90</v>
+      </c>
+      <c r="B38">
+        <v>37.783499999999997</v>
+      </c>
+      <c r="C38">
+        <v>-122.4158</v>
+      </c>
+      <c r="D38">
+        <v>0.44235000000000002</v>
+      </c>
+      <c r="E38" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>91</v>
+      </c>
+      <c r="B39">
+        <v>37.791499999999999</v>
+      </c>
+      <c r="C39">
+        <v>-122.39879999999999</v>
+      </c>
+      <c r="D39">
+        <v>0.49914999999999998</v>
+      </c>
+      <c r="E39" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>92</v>
+      </c>
+      <c r="B40">
+        <v>37.717799999999997</v>
+      </c>
+      <c r="C40">
+        <v>-122.4622</v>
+      </c>
+      <c r="D40">
+        <v>7.6637999999999998E-2</v>
+      </c>
+      <c r="E40" t="s">
+        <v>93</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A6:AJ87"/>
   <sheetViews>
     <sheetView topLeftCell="A64" workbookViewId="0">
@@ -6061,7 +6726,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AO36"/>
   <sheetViews>
@@ -10577,7 +11242,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H1226"/>
   <sheetViews>
@@ -42469,7 +43134,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I1226"/>
   <sheetViews>
@@ -78820,7 +79485,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L24" sqref="L24"/>
     </sheetView>
   </sheetViews>
@@ -79938,6 +80603,208 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B2" t="s">
+        <v>141</v>
+      </c>
+      <c r="C2">
+        <v>2868</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>142</v>
+      </c>
+      <c r="B3" t="s">
+        <v>143</v>
+      </c>
+      <c r="C3">
+        <v>2060</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>143</v>
+      </c>
+      <c r="B4" t="s">
+        <v>142</v>
+      </c>
+      <c r="C4">
+        <v>16145</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>141</v>
+      </c>
+      <c r="B5" t="s">
+        <v>140</v>
+      </c>
+      <c r="C5">
+        <v>1013</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>140</v>
+      </c>
+      <c r="B6" t="s">
+        <v>143</v>
+      </c>
+      <c r="C6">
+        <v>8916</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>142</v>
+      </c>
+      <c r="B7" t="s">
+        <v>142</v>
+      </c>
+      <c r="C7">
+        <v>10048</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>143</v>
+      </c>
+      <c r="B8" t="s">
+        <v>140</v>
+      </c>
+      <c r="C8">
+        <v>8010</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>141</v>
+      </c>
+      <c r="B9" t="s">
+        <v>141</v>
+      </c>
+      <c r="C9">
+        <v>6907</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>140</v>
+      </c>
+      <c r="B10" t="s">
+        <v>142</v>
+      </c>
+      <c r="C10">
+        <v>5871</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>142</v>
+      </c>
+      <c r="B11" t="s">
+        <v>140</v>
+      </c>
+      <c r="C11">
+        <v>1951</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>143</v>
+      </c>
+      <c r="B12" t="s">
+        <v>141</v>
+      </c>
+      <c r="C12">
+        <v>8045</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>141</v>
+      </c>
+      <c r="B13" t="s">
+        <v>143</v>
+      </c>
+      <c r="C13">
+        <v>940</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>140</v>
+      </c>
+      <c r="B14" t="s">
+        <v>140</v>
+      </c>
+      <c r="C14">
+        <v>11975</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>142</v>
+      </c>
+      <c r="B15" t="s">
+        <v>141</v>
+      </c>
+      <c r="C15">
+        <v>6171</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>143</v>
+      </c>
+      <c r="B16" t="s">
+        <v>143</v>
+      </c>
+      <c r="C16">
+        <v>8090</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>141</v>
+      </c>
+      <c r="B17" t="s">
+        <v>142</v>
+      </c>
+      <c r="C17">
+        <v>990</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F65"/>
   <sheetViews>
@@ -81255,647 +82122,4 @@
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E40"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:E40"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>45</v>
-      </c>
-      <c r="B5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C5" t="s">
-        <v>47</v>
-      </c>
-      <c r="D5" t="s">
-        <v>48</v>
-      </c>
-      <c r="E5" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>50</v>
-      </c>
-      <c r="B6">
-        <v>37.724400000000003</v>
-      </c>
-      <c r="C6">
-        <v>-122.42100000000001</v>
-      </c>
-      <c r="D6">
-        <v>8.3884E-2</v>
-      </c>
-      <c r="E6" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>52</v>
-      </c>
-      <c r="B7">
-        <v>37.710700000000003</v>
-      </c>
-      <c r="C7">
-        <v>-122.4372</v>
-      </c>
-      <c r="D7">
-        <v>5.8438999999999998E-2</v>
-      </c>
-      <c r="E7" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>54</v>
-      </c>
-      <c r="B8">
-        <v>37.802100000000003</v>
-      </c>
-      <c r="C8">
-        <v>-122.43689999999999</v>
-      </c>
-      <c r="D8">
-        <v>0.40364</v>
-      </c>
-      <c r="E8" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>56</v>
-      </c>
-      <c r="B9">
-        <v>37.792999999999999</v>
-      </c>
-      <c r="C9">
-        <v>-122.416</v>
-      </c>
-      <c r="D9">
-        <v>0.33259</v>
-      </c>
-      <c r="E9" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>57</v>
-      </c>
-      <c r="B10">
-        <v>37.804499999999997</v>
-      </c>
-      <c r="C10">
-        <v>-122.4076</v>
-      </c>
-      <c r="D10">
-        <v>0.28783999999999998</v>
-      </c>
-      <c r="E10" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>58</v>
-      </c>
-      <c r="B11">
-        <v>37.792400000000001</v>
-      </c>
-      <c r="C11">
-        <v>-122.43519999999999</v>
-      </c>
-      <c r="D11">
-        <v>0.33382000000000001</v>
-      </c>
-      <c r="E11" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>59</v>
-      </c>
-      <c r="B12">
-        <v>37.786799999999999</v>
-      </c>
-      <c r="C12">
-        <v>-122.4538</v>
-      </c>
-      <c r="D12">
-        <v>0.19964999999999999</v>
-      </c>
-      <c r="E12" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>60</v>
-      </c>
-      <c r="B13">
-        <v>37.801400000000001</v>
-      </c>
-      <c r="C13">
-        <v>-122.4182</v>
-      </c>
-      <c r="D13">
-        <v>0.34165000000000001</v>
-      </c>
-      <c r="E13" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>61</v>
-      </c>
-      <c r="B14">
-        <v>37.714399999999998</v>
-      </c>
-      <c r="C14">
-        <v>-122.4113</v>
-      </c>
-      <c r="D14">
-        <v>6.4773999999999998E-2</v>
-      </c>
-      <c r="E14" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>63</v>
-      </c>
-      <c r="B15">
-        <v>37.7423</v>
-      </c>
-      <c r="C15">
-        <v>-122.4423</v>
-      </c>
-      <c r="D15">
-        <v>7.4148000000000006E-2</v>
-      </c>
-      <c r="E15" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>65</v>
-      </c>
-      <c r="B16">
-        <v>37.7378</v>
-      </c>
-      <c r="C16">
-        <v>-122.4316</v>
-      </c>
-      <c r="D16">
-        <v>0.1226</v>
-      </c>
-      <c r="E16" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>66</v>
-      </c>
-      <c r="B17">
-        <v>37.758400000000002</v>
-      </c>
-      <c r="C17">
-        <v>-122.4654</v>
-      </c>
-      <c r="D17">
-        <v>0.18995000000000001</v>
-      </c>
-      <c r="E17" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>67</v>
-      </c>
-      <c r="B18">
-        <v>37.722499999999997</v>
-      </c>
-      <c r="C18">
-        <v>-122.4885</v>
-      </c>
-      <c r="D18">
-        <v>9.2602000000000004E-2</v>
-      </c>
-      <c r="E18" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>68</v>
-      </c>
-      <c r="B19">
-        <v>37.7239</v>
-      </c>
-      <c r="C19">
-        <v>-122.4439</v>
-      </c>
-      <c r="D19">
-        <v>0.10242</v>
-      </c>
-      <c r="E19" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>69</v>
-      </c>
-      <c r="B20">
-        <v>37.737299999999998</v>
-      </c>
-      <c r="C20">
-        <v>-122.4589</v>
-      </c>
-      <c r="D20">
-        <v>0.12472999999999999</v>
-      </c>
-      <c r="E20" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>70</v>
-      </c>
-      <c r="B21">
-        <v>37.729999999999997</v>
-      </c>
-      <c r="C21">
-        <v>-122.38549999999999</v>
-      </c>
-      <c r="D21">
-        <v>0.10309</v>
-      </c>
-      <c r="E21" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>72</v>
-      </c>
-      <c r="B22">
-        <v>37.739899999999999</v>
-      </c>
-      <c r="C22">
-        <v>-122.4169</v>
-      </c>
-      <c r="D22">
-        <v>0.20043</v>
-      </c>
-      <c r="E22" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>73</v>
-      </c>
-      <c r="B23">
-        <v>37.7624</v>
-      </c>
-      <c r="C23">
-        <v>-122.4348</v>
-      </c>
-      <c r="D23">
-        <v>0.34092</v>
-      </c>
-      <c r="E23" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>74</v>
-      </c>
-      <c r="B24">
-        <v>37.769199999999998</v>
-      </c>
-      <c r="C24">
-        <v>-122.44629999999999</v>
-      </c>
-      <c r="D24">
-        <v>0.29559000000000002</v>
-      </c>
-      <c r="E24" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>75</v>
-      </c>
-      <c r="B25">
-        <v>37.758899999999997</v>
-      </c>
-      <c r="C25">
-        <v>-122.4153</v>
-      </c>
-      <c r="D25">
-        <v>0.42582999999999999</v>
-      </c>
-      <c r="E25" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>76</v>
-      </c>
-      <c r="B26">
-        <v>37.749299999999998</v>
-      </c>
-      <c r="C26">
-        <v>-122.43300000000001</v>
-      </c>
-      <c r="D26">
-        <v>0.25158000000000003</v>
-      </c>
-      <c r="E26" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>77</v>
-      </c>
-      <c r="B27">
-        <v>37.741100000000003</v>
-      </c>
-      <c r="C27">
-        <v>-122.4892</v>
-      </c>
-      <c r="D27">
-        <v>9.2271000000000006E-2</v>
-      </c>
-      <c r="E27" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>78</v>
-      </c>
-      <c r="B28">
-        <v>37.758299999999998</v>
-      </c>
-      <c r="C28">
-        <v>-122.393</v>
-      </c>
-      <c r="D28">
-        <v>0.26352999999999999</v>
-      </c>
-      <c r="E28" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>79</v>
-      </c>
-      <c r="B29">
-        <v>37.776400000000002</v>
-      </c>
-      <c r="C29">
-        <v>-122.3994</v>
-      </c>
-      <c r="D29">
-        <v>0.55315999999999999</v>
-      </c>
-      <c r="E29" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>80</v>
-      </c>
-      <c r="B30">
-        <v>37.752000000000002</v>
-      </c>
-      <c r="C30">
-        <v>-122.45</v>
-      </c>
-      <c r="D30">
-        <v>0.13105</v>
-      </c>
-      <c r="E30" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>81</v>
-      </c>
-      <c r="B31">
-        <v>37.7804</v>
-      </c>
-      <c r="C31">
-        <v>-122.4332</v>
-      </c>
-      <c r="D31">
-        <v>0.41192000000000001</v>
-      </c>
-      <c r="E31" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>82</v>
-      </c>
-      <c r="B32">
-        <v>37.780200000000001</v>
-      </c>
-      <c r="C32">
-        <v>-122.4652</v>
-      </c>
-      <c r="D32">
-        <v>0.21193999999999999</v>
-      </c>
-      <c r="E32" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>84</v>
-      </c>
-      <c r="B33">
-        <v>37.777999999999999</v>
-      </c>
-      <c r="C33">
-        <v>-122.4928</v>
-      </c>
-      <c r="D33">
-        <v>0.18915999999999999</v>
-      </c>
-      <c r="E33" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>85</v>
-      </c>
-      <c r="B34">
-        <v>37.755299999999998</v>
-      </c>
-      <c r="C34">
-        <v>-122.49379999999999</v>
-      </c>
-      <c r="D34">
-        <v>0.12363</v>
-      </c>
-      <c r="E34" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>86</v>
-      </c>
-      <c r="B35">
-        <v>37.784100000000002</v>
-      </c>
-      <c r="C35">
-        <v>-122.5009</v>
-      </c>
-      <c r="D35">
-        <v>9.1937000000000005E-2</v>
-      </c>
-      <c r="E35" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>87</v>
-      </c>
-      <c r="B36">
-        <v>37.768900000000002</v>
-      </c>
-      <c r="C36">
-        <v>-122.4828</v>
-      </c>
-      <c r="D36">
-        <v>0.15941</v>
-      </c>
-      <c r="E36" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>88</v>
-      </c>
-      <c r="B37">
-        <v>37.7941</v>
-      </c>
-      <c r="C37">
-        <v>-122.407</v>
-      </c>
-      <c r="D37">
-        <v>0.24273</v>
-      </c>
-      <c r="E37" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>90</v>
-      </c>
-      <c r="B38">
-        <v>37.783499999999997</v>
-      </c>
-      <c r="C38">
-        <v>-122.4158</v>
-      </c>
-      <c r="D38">
-        <v>0.44235000000000002</v>
-      </c>
-      <c r="E38" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>91</v>
-      </c>
-      <c r="B39">
-        <v>37.791499999999999</v>
-      </c>
-      <c r="C39">
-        <v>-122.39879999999999</v>
-      </c>
-      <c r="D39">
-        <v>0.49914999999999998</v>
-      </c>
-      <c r="E39" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>92</v>
-      </c>
-      <c r="B40">
-        <v>37.717799999999997</v>
-      </c>
-      <c r="C40">
-        <v>-122.4622</v>
-      </c>
-      <c r="D40">
-        <v>7.6637999999999998E-2</v>
-      </c>
-      <c r="E40" t="s">
-        <v>93</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>